<commit_message>
Code for Streamgraphs of Timeseries
</commit_message>
<xml_diff>
--- a/data/SarmientoPublications.xlsx
+++ b/data/SarmientoPublications.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="389">
   <si>
     <t>Broecker, W.S., J. Goddard, and J.L. Sarmiento, 1976. The distribution of 226Ra in the Atlantic Ocean. Earth Planet. Sci. Lett., 32, 220-235.</t>
   </si>
@@ -726,9 +726,6 @@
     <t>CO2, phosphorus, nitrogen, macroalgae</t>
   </si>
   <si>
-    <t>Chemcial</t>
-  </si>
-  <si>
     <t>nitrogen, chlorophyll, carbon, nitrate</t>
   </si>
   <si>
@@ -805,9 +802,6 @@
   </si>
   <si>
     <t>Iglesias-Rodriguez, M. D., R. Armstrong, R. Feely, R. Hood, J. Kleypas, J. D. Milliman, C. Sabine, and J. Sarmiento, 2002. Progress made in study of ocean's calcium carbonate budget.   EOS Transactions, 83 (34): 365, 374-375.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chemical </t>
   </si>
   <si>
     <t>CaCO3, CO2, calcite, aragonite, calcifying phytoplankton, zooplankton</t>
@@ -1794,8 +1788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="E98" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1814,7 +1808,7 @@
         <v>196</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>198</v>
@@ -1834,7 +1828,7 @@
         <v>1976</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D2" t="s">
         <v>199</v>
@@ -1854,7 +1848,7 @@
         <v>1976</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D3" t="s">
         <v>199</v>
@@ -1874,7 +1868,7 @@
         <v>1976</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E4" t="s">
         <v>204</v>
@@ -1891,7 +1885,7 @@
         <v>1978</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D5" t="s">
         <v>199</v>
@@ -1911,7 +1905,7 @@
         <v>1980</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D6" t="s">
         <v>199</v>
@@ -1931,7 +1925,7 @@
         <v>1980</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D7" t="s">
         <v>199</v>
@@ -1957,7 +1951,7 @@
         <v>1982</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E9" t="s">
         <v>203</v>
@@ -1971,7 +1965,7 @@
         <v>1982</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D10" t="s">
         <v>199</v>
@@ -1991,7 +1985,7 @@
         <v>1982</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D11" t="s">
         <v>199</v>
@@ -2011,7 +2005,7 @@
         <v>1983</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E12" t="s">
         <v>203</v>
@@ -2028,7 +2022,7 @@
         <v>1983</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E13" t="s">
         <v>203</v>
@@ -2045,7 +2039,7 @@
         <v>1984</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E14" t="s">
         <v>204</v>
@@ -2062,7 +2056,7 @@
         <v>1985</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E15" t="s">
         <v>203</v>
@@ -2076,7 +2070,7 @@
         <v>1985</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D16" t="s">
         <v>199</v>
@@ -2096,7 +2090,7 @@
         <v>1985</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E17" t="s">
         <v>204</v>
@@ -2113,7 +2107,7 @@
         <v>1985</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D18" t="s">
         <v>209</v>
@@ -2133,7 +2127,7 @@
         <v>1985</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D19" t="s">
         <v>212</v>
@@ -2153,13 +2147,13 @@
         <v>1985</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E20" t="s">
         <v>204</v>
       </c>
       <c r="F20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="48">
@@ -2170,7 +2164,7 @@
         <v>1986</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E21" t="s">
         <v>203</v>
@@ -2187,7 +2181,7 @@
         <v>1986</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E22" t="s">
         <v>203</v>
@@ -2204,7 +2198,7 @@
         <v>1986</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E23" t="s">
         <v>203</v>
@@ -2221,7 +2215,7 @@
         <v>1986</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E24" t="s">
         <v>204</v>
@@ -2238,7 +2232,7 @@
         <v>1986</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D25" t="s">
         <v>212</v>
@@ -2258,7 +2252,7 @@
         <v>1986</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E26" t="s">
         <v>203</v>
@@ -2272,7 +2266,7 @@
         <v>1986</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E27" t="s">
         <v>204</v>
@@ -2289,7 +2283,7 @@
         <v>1986</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E28" t="s">
         <v>203</v>
@@ -2303,7 +2297,7 @@
         <v>1986</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E29" t="s">
         <v>204</v>
@@ -2320,7 +2314,7 @@
         <v>1987</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D30" t="s">
         <v>212</v>
@@ -2340,7 +2334,7 @@
         <v>1988</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E31" t="s">
         <v>204</v>
@@ -2357,7 +2351,7 @@
         <v>1988</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E32" t="s">
         <v>204</v>
@@ -2374,13 +2368,13 @@
         <v>1988</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E33" t="s">
         <v>227</v>
       </c>
       <c r="F33" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="48">
@@ -2391,7 +2385,7 @@
         <v>1988</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E34" t="s">
         <v>204</v>
@@ -2408,7 +2402,7 @@
         <v>1989</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E35" t="s">
         <v>204</v>
@@ -2425,7 +2419,7 @@
         <v>1990</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E36" t="s">
         <v>203</v>
@@ -2442,7 +2436,7 @@
         <v>1990</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E37" t="s">
         <v>204</v>
@@ -2459,7 +2453,7 @@
         <v>1990</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E38" t="s">
         <v>204</v>
@@ -2476,7 +2470,7 @@
         <v>1991</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E39" t="s">
         <v>204</v>
@@ -2493,7 +2487,7 @@
         <v>1991</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E40" t="s">
         <v>204</v>
@@ -2510,7 +2504,7 @@
         <v>1991</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E41" t="s">
         <v>227</v>
@@ -2527,7 +2521,7 @@
         <v>1991</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E42" t="s">
         <v>204</v>
@@ -2544,7 +2538,7 @@
         <v>1991</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E43" t="s">
         <v>204</v>
@@ -2561,7 +2555,7 @@
         <v>1991</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E44" t="s">
         <v>203</v>
@@ -2578,7 +2572,7 @@
         <v>1991</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E45" t="s">
         <v>204</v>
@@ -2595,7 +2589,7 @@
         <v>1992</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E46" t="s">
         <v>204</v>
@@ -2612,7 +2606,7 @@
         <v>1992</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E47" t="s">
         <v>204</v>
@@ -2629,7 +2623,7 @@
         <v>1992</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E48" t="s">
         <v>204</v>
@@ -2646,7 +2640,7 @@
         <v>1992</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E49" t="s">
         <v>204</v>
@@ -2663,7 +2657,7 @@
         <v>1992</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E50" t="s">
         <v>204</v>
@@ -2680,13 +2674,13 @@
         <v>1992</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E51" t="s">
         <v>204</v>
       </c>
       <c r="F51" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="32">
@@ -2697,7 +2691,7 @@
         <v>1993</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E52" t="s">
         <v>204</v>
@@ -2714,13 +2708,13 @@
         <v>1993</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E53" t="s">
         <v>204</v>
       </c>
       <c r="F53" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="64">
@@ -2731,13 +2725,13 @@
         <v>1993</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E54" t="s">
         <v>227</v>
       </c>
       <c r="F54" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="32">
@@ -2748,7 +2742,7 @@
         <v>1993</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E55" t="s">
         <v>204</v>
@@ -2765,7 +2759,7 @@
         <v>1993</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E56" t="s">
         <v>204</v>
@@ -2782,16 +2776,16 @@
         <v>1993</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D57" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E57" t="s">
         <v>227</v>
       </c>
       <c r="F57" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="48">
@@ -2802,13 +2796,13 @@
         <v>1994</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E58" t="s">
         <v>204</v>
       </c>
       <c r="F58" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="48">
@@ -2819,13 +2813,13 @@
         <v>1994</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E59" t="s">
         <v>227</v>
       </c>
       <c r="F59" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="48">
@@ -2836,7 +2830,7 @@
         <v>1994</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E60" t="s">
         <v>204</v>
@@ -2850,7 +2844,7 @@
         <v>58</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="64">
@@ -2861,13 +2855,13 @@
         <v>1995</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E62" t="s">
         <v>203</v>
       </c>
       <c r="F62" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="48">
@@ -2878,10 +2872,10 @@
         <v>1995</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E63" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="F63" t="s">
         <v>207</v>
@@ -2895,13 +2889,13 @@
         <v>1995</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E64" t="s">
         <v>227</v>
       </c>
       <c r="F64" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="32">
@@ -2918,13 +2912,13 @@
         <v>1995</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E66" t="s">
         <v>204</v>
       </c>
       <c r="F66" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="48">
@@ -2935,13 +2929,13 @@
         <v>1995</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E67" t="s">
         <v>204</v>
       </c>
       <c r="F67" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="64">
@@ -2952,13 +2946,13 @@
         <v>1996</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E68" t="s">
         <v>204</v>
       </c>
       <c r="F68" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="48">
@@ -2969,7 +2963,7 @@
         <v>1996</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D69" t="s">
         <v>209</v>
@@ -2989,7 +2983,7 @@
         <v>1996</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E70" t="s">
         <v>204</v>
@@ -3006,13 +3000,13 @@
         <v>1996</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E71" t="s">
         <v>204</v>
       </c>
       <c r="F71" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="48">
@@ -3023,7 +3017,7 @@
         <v>1997</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D72" t="s">
         <v>199</v>
@@ -3032,7 +3026,7 @@
         <v>204</v>
       </c>
       <c r="F72" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="48">
@@ -3043,7 +3037,7 @@
         <v>1998</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E73" t="s">
         <v>204</v>
@@ -3060,7 +3054,7 @@
         <v>1998</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E74" t="s">
         <v>204</v>
@@ -3077,10 +3071,10 @@
         <v>1999</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D75" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E75" t="s">
         <v>204</v>
@@ -3097,7 +3091,7 @@
         <v>1998</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E76" t="s">
         <v>204</v>
@@ -3114,7 +3108,7 @@
         <v>1999</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E77" t="s">
         <v>204</v>
@@ -3131,7 +3125,7 @@
         <v>1999</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E78" t="s">
         <v>204</v>
@@ -3148,7 +3142,7 @@
         <v>1999</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E79" t="s">
         <v>204</v>
@@ -3165,7 +3159,7 @@
         <v>1999</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E80" t="s">
         <v>204</v>
@@ -3182,7 +3176,7 @@
         <v>1999</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E81" t="s">
         <v>204</v>
@@ -3199,13 +3193,13 @@
         <v>2000</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E82" t="s">
         <v>204</v>
       </c>
       <c r="F82" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="64">
@@ -3216,10 +3210,10 @@
         <v>2000</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D83" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E83" t="s">
         <v>204</v>
@@ -3236,13 +3230,13 @@
         <v>2000</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E84" t="s">
         <v>204</v>
       </c>
       <c r="F84" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="32">
@@ -3253,7 +3247,7 @@
         <v>2000</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E85" t="s">
         <v>204</v>
@@ -3270,10 +3264,10 @@
         <v>2000</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D86" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E86" t="s">
         <v>204</v>
@@ -3284,39 +3278,39 @@
     </row>
     <row r="87" spans="1:6" ht="64">
       <c r="A87" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B87">
         <v>2000</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E87" t="s">
         <v>204</v>
       </c>
       <c r="F87" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="96">
       <c r="A88" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B88">
         <v>2001</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D88" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E88" t="s">
         <v>204</v>
       </c>
       <c r="F88" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="48">
@@ -3327,16 +3321,16 @@
         <v>2001</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D89" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E89" t="s">
         <v>204</v>
       </c>
       <c r="F89" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="112">
@@ -3347,7 +3341,7 @@
         <v>2001</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E90" t="s">
         <v>204</v>
@@ -3364,16 +3358,16 @@
         <v>2001</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D91" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E91" t="s">
         <v>203</v>
       </c>
       <c r="F91" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="64">
@@ -3384,13 +3378,13 @@
         <v>2001</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E92" t="s">
         <v>204</v>
       </c>
       <c r="F92" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="64">
@@ -3401,13 +3395,13 @@
         <v>2002</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E93" t="s">
         <v>203</v>
       </c>
       <c r="F93" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="48">
@@ -3418,10 +3412,10 @@
         <v>2002</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D94" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E94" t="s">
         <v>204</v>
@@ -3432,33 +3426,33 @@
     </row>
     <row r="95" spans="1:6" ht="80">
       <c r="A95" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B95">
         <v>2002</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E95" t="s">
         <v>204</v>
       </c>
       <c r="F95" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="128">
       <c r="A96" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B96">
         <v>2002</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D96" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E96" t="s">
         <v>204</v>
@@ -3475,16 +3469,16 @@
         <v>2002</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D97" t="s">
+        <v>256</v>
+      </c>
+      <c r="E97" t="s">
+        <v>204</v>
+      </c>
+      <c r="F97" t="s">
         <v>257</v>
-      </c>
-      <c r="E97" t="s">
-        <v>204</v>
-      </c>
-      <c r="F97" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="80">
@@ -3495,13 +3489,13 @@
         <v>2002</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E98" t="s">
         <v>204</v>
       </c>
       <c r="F98" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="64">
@@ -3512,13 +3506,13 @@
         <v>2002</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E99" t="s">
         <v>204</v>
       </c>
       <c r="F99" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="32">
@@ -3529,7 +3523,7 @@
         <v>2002</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E100" t="s">
         <v>204</v>
@@ -3540,19 +3534,19 @@
     </row>
     <row r="101" spans="1:6" ht="64">
       <c r="A101" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B101">
         <v>2002</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E101" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="F101" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="64">
@@ -3563,7 +3557,7 @@
         <v>2002</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E102" t="s">
         <v>204</v>
@@ -3580,24 +3574,24 @@
         <v>2002</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E103" t="s">
         <v>204</v>
       </c>
       <c r="F103" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="80">
       <c r="A104" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B104">
         <v>2003</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E104" t="s">
         <v>204</v>
@@ -3614,13 +3608,13 @@
         <v>2003</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E105" t="s">
         <v>204</v>
       </c>
       <c r="F105" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="80">
@@ -3631,7 +3625,7 @@
         <v>2003</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E106" t="s">
         <v>204</v>
@@ -3648,30 +3642,30 @@
         <v>2003</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E107" t="s">
         <v>204</v>
       </c>
       <c r="F107" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="64">
       <c r="A108" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B108">
         <v>2003</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E108" t="s">
         <v>204</v>
       </c>
       <c r="F108" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="64">
@@ -3682,10 +3676,10 @@
         <v>2003</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D109" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E109" t="s">
         <v>204</v>
@@ -3702,10 +3696,10 @@
         <v>2003</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D110" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E110" t="s">
         <v>204</v>
@@ -3722,10 +3716,10 @@
         <v>2003</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D111" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E111" t="s">
         <v>204</v>
@@ -3742,10 +3736,10 @@
         <v>2003</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D112" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E112" t="s">
         <v>204</v>
@@ -3762,13 +3756,13 @@
         <v>2003</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E113" t="s">
         <v>204</v>
       </c>
       <c r="F113" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="160">
@@ -3779,10 +3773,10 @@
         <v>2003</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D114" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E114" t="s">
         <v>204</v>
@@ -3799,13 +3793,13 @@
         <v>2004</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E115" t="s">
         <v>204</v>
       </c>
       <c r="F115" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="144">
@@ -3816,16 +3810,16 @@
         <v>2004</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D116" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E116" t="s">
         <v>204</v>
       </c>
       <c r="F116" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="48">
@@ -3836,7 +3830,7 @@
         <v>2004</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E117" t="s">
         <v>204</v>
@@ -3853,13 +3847,13 @@
         <v>2004</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E118" t="s">
         <v>204</v>
       </c>
       <c r="F118" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="64">
@@ -3870,10 +3864,10 @@
         <v>2004</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E119" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F119" t="s">
         <v>207</v>
@@ -3887,13 +3881,13 @@
         <v>2004</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E120" t="s">
         <v>227</v>
       </c>
       <c r="F120" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="64">
@@ -3901,10 +3895,10 @@
         <v>111</v>
       </c>
       <c r="B121" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="144">
@@ -3915,16 +3909,16 @@
         <v>2004</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D122" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E122" t="s">
         <v>203</v>
       </c>
       <c r="F122" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="96">
@@ -3935,13 +3929,13 @@
         <v>2004</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E123" t="s">
         <v>203</v>
       </c>
       <c r="F123" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="128">
@@ -3952,13 +3946,13 @@
         <v>2005</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E124" t="s">
         <v>227</v>
       </c>
       <c r="F124" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="64">
@@ -3969,13 +3963,13 @@
         <v>2005</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E125" t="s">
         <v>204</v>
       </c>
       <c r="F125" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="80">
@@ -3986,7 +3980,7 @@
         <v>2006</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E126" t="s">
         <v>204</v>
@@ -4003,13 +3997,13 @@
         <v>2006</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E127" t="s">
         <v>204</v>
       </c>
       <c r="F127" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="144">
@@ -4020,7 +4014,7 @@
         <v>2006</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E128" t="s">
         <v>204</v>
@@ -4037,13 +4031,13 @@
         <v>2006</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E129" t="s">
         <v>204</v>
       </c>
       <c r="F129" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="130" spans="1:6" ht="48">
@@ -4054,7 +4048,7 @@
         <v>2006</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E130" t="s">
         <v>204</v>
@@ -4071,10 +4065,10 @@
         <v>2006</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D131" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E131" t="s">
         <v>204</v>
@@ -4091,13 +4085,13 @@
         <v>2006</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E132" t="s">
         <v>227</v>
       </c>
       <c r="F132" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="48">
@@ -4108,27 +4102,27 @@
         <v>2007</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E133" t="s">
         <v>204</v>
       </c>
       <c r="F133" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="112">
       <c r="A134" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B134">
         <v>2007</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D134" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E134" t="s">
         <v>204</v>
@@ -4145,7 +4139,7 @@
         <v>2007</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E135" t="s">
         <v>204</v>
@@ -4156,13 +4150,13 @@
     </row>
     <row r="136" spans="1:6" ht="80">
       <c r="A136" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B136">
         <v>2007</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E136" t="s">
         <v>204</v>
@@ -4179,13 +4173,13 @@
         <v>2007</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E137" t="s">
         <v>204</v>
       </c>
       <c r="F137" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="112">
@@ -4196,16 +4190,16 @@
         <v>2007</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D138" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E138" t="s">
         <v>204</v>
       </c>
       <c r="F138" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="139" spans="1:6" ht="80">
@@ -4216,13 +4210,13 @@
         <v>2007</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E139" t="s">
         <v>204</v>
       </c>
       <c r="F139" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="140" spans="1:6" ht="160">
@@ -4233,16 +4227,16 @@
         <v>2007</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D140" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E140" t="s">
         <v>204</v>
       </c>
       <c r="F140" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="141" spans="1:6" ht="160">
@@ -4253,7 +4247,7 @@
         <v>2007</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E141" t="s">
         <v>204</v>
@@ -4270,13 +4264,13 @@
         <v>2007</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E142" t="s">
         <v>204</v>
       </c>
       <c r="F142" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="64">
@@ -4287,10 +4281,10 @@
         <v>2008</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E143" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="F143" t="s">
         <v>207</v>
@@ -4304,13 +4298,13 @@
         <v>2008</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E144" t="s">
         <v>204</v>
       </c>
       <c r="F144" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="48">
@@ -4321,13 +4315,13 @@
         <v>2008</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E145" t="s">
         <v>204</v>
       </c>
       <c r="F145" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="64">
@@ -4338,7 +4332,7 @@
         <v>2008</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E146" t="s">
         <v>204</v>
@@ -4355,13 +4349,13 @@
         <v>2008</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E147" t="s">
         <v>204</v>
       </c>
       <c r="F147" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="148" spans="1:6" ht="64">
@@ -4372,13 +4366,13 @@
         <v>2008</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E148" t="s">
         <v>204</v>
       </c>
       <c r="F148" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="149" spans="1:6" ht="80">
@@ -4389,13 +4383,13 @@
         <v>2009</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E149" t="s">
         <v>227</v>
       </c>
       <c r="F149" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="150" spans="1:6" ht="96">
@@ -4406,7 +4400,7 @@
         <v>2009</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E150" t="s">
         <v>204</v>
@@ -4423,13 +4417,13 @@
         <v>2009</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E151" t="s">
         <v>227</v>
       </c>
       <c r="F151" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="152" spans="1:6" ht="112">
@@ -4440,13 +4434,13 @@
         <v>2009</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E152" t="s">
         <v>227</v>
       </c>
       <c r="F152" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="153" spans="1:6" ht="48">
@@ -4457,13 +4451,13 @@
         <v>2009</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E153" t="s">
         <v>204</v>
       </c>
       <c r="F153" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="154" spans="1:6" ht="128">
@@ -4474,13 +4468,13 @@
         <v>2009</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E154" t="s">
         <v>204</v>
       </c>
       <c r="F154" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="155" spans="1:6" ht="176">
@@ -4491,7 +4485,7 @@
         <v>2009</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E155" t="s">
         <v>204</v>
@@ -4508,13 +4502,13 @@
         <v>2010</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E156" t="s">
         <v>227</v>
       </c>
       <c r="F156" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="64">
@@ -4525,13 +4519,13 @@
         <v>2010</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E157" t="s">
         <v>227</v>
       </c>
       <c r="F157" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="64">
@@ -4542,7 +4536,7 @@
         <v>2010</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E158" t="s">
         <v>204</v>
@@ -4559,7 +4553,7 @@
         <v>2010</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E159" t="s">
         <v>204</v>
@@ -4576,13 +4570,13 @@
         <v>2010</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E160" t="s">
         <v>204</v>
       </c>
       <c r="F160" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="64">
@@ -4593,13 +4587,13 @@
         <v>2010</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E161" t="s">
         <v>204</v>
       </c>
       <c r="F161" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="80">
@@ -4610,13 +4604,13 @@
         <v>2010</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E162" t="s">
         <v>204</v>
       </c>
       <c r="F162" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="64">
@@ -4627,13 +4621,13 @@
         <v>2010</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E163" t="s">
         <v>204</v>
       </c>
       <c r="F163" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="128">
@@ -4644,30 +4638,30 @@
         <v>2010</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E164" t="s">
         <v>227</v>
       </c>
       <c r="F164" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="80">
       <c r="A165" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B165">
         <v>2011</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E165" t="s">
         <v>227</v>
       </c>
       <c r="F165" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="166" spans="1:6" ht="64">
@@ -4678,7 +4672,7 @@
         <v>2011</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E166" t="s">
         <v>203</v>
@@ -4692,13 +4686,13 @@
         <v>2011</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E167" t="s">
         <v>203</v>
       </c>
       <c r="F167" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="80">
@@ -4709,13 +4703,13 @@
         <v>2011</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E168" t="s">
         <v>204</v>
       </c>
       <c r="F168" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="80">
@@ -4726,13 +4720,13 @@
         <v>2011</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E169" t="s">
         <v>227</v>
       </c>
       <c r="F169" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="96">
@@ -4743,13 +4737,13 @@
         <v>2011</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E170" t="s">
         <v>203</v>
       </c>
       <c r="F170" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="64">
@@ -4760,7 +4754,7 @@
         <v>2011</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E171" t="s">
         <v>203</v>
@@ -4774,7 +4768,7 @@
         <v>2012</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E172" t="s">
         <v>204</v>
@@ -4791,10 +4785,10 @@
         <v>2012</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E173" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="80">
@@ -4805,13 +4799,13 @@
         <v>2012</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E174" t="s">
         <v>204</v>
       </c>
       <c r="F174" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="80">
@@ -4822,13 +4816,13 @@
         <v>2012</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E175" t="s">
         <v>227</v>
       </c>
       <c r="F175" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="80">
@@ -4839,13 +4833,13 @@
         <v>2012</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E176" t="s">
         <v>203</v>
       </c>
       <c r="F176" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="177" spans="1:6" ht="96">
@@ -4856,13 +4850,13 @@
         <v>2012</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E177" t="s">
         <v>204</v>
       </c>
       <c r="F177" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="80">
@@ -4873,13 +4867,13 @@
         <v>2012</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E178" t="s">
         <v>227</v>
       </c>
       <c r="F178" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="80">
@@ -4890,13 +4884,13 @@
         <v>2013</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E179" t="s">
         <v>227</v>
       </c>
       <c r="F179" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="180" spans="1:6" ht="64">
@@ -4907,7 +4901,7 @@
         <v>2013</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E180" t="s">
         <v>204</v>
@@ -4924,13 +4918,13 @@
         <v>2013</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E181" t="s">
         <v>227</v>
       </c>
       <c r="F181" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="182" spans="1:6" ht="64">
@@ -4941,7 +4935,7 @@
         <v>2013</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E182" t="s">
         <v>203</v>
@@ -4958,7 +4952,7 @@
         <v>2013</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E183" t="s">
         <v>203</v>
@@ -4972,7 +4966,7 @@
         <v>2013</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E184" t="s">
         <v>204</v>
@@ -4989,13 +4983,13 @@
         <v>2013</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E185" t="s">
         <v>204</v>
       </c>
       <c r="F185" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="112">
@@ -5006,10 +5000,10 @@
         <v>2013</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E186" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="96">
@@ -5020,7 +5014,7 @@
         <v>2013</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E187" t="s">
         <v>204</v>
@@ -5034,13 +5028,13 @@
         <v>2013</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E188" t="s">
         <v>227</v>
       </c>
       <c r="F188" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="189" spans="1:6" ht="64">
@@ -5051,13 +5045,13 @@
         <v>2013</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E189" t="s">
         <v>227</v>
       </c>
       <c r="F189" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="190" spans="1:6" ht="64">
@@ -5068,13 +5062,13 @@
         <v>2013</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E190" t="s">
         <v>227</v>
       </c>
       <c r="F190" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="48">
@@ -5085,7 +5079,7 @@
         <v>2013</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E191" t="s">
         <v>203</v>
@@ -5102,7 +5096,7 @@
         <v>2014</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E192" t="s">
         <v>204</v>
@@ -5119,13 +5113,13 @@
         <v>2014</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E193" t="s">
         <v>227</v>
       </c>
       <c r="F193" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="194" spans="1:6" ht="64">
@@ -5136,7 +5130,7 @@
         <v>2014</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E194" t="s">
         <v>204</v>
@@ -5153,7 +5147,7 @@
         <v>2014</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E195" t="s">
         <v>204</v>
@@ -5170,7 +5164,7 @@
         <v>2014</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E196" t="s">
         <v>204</v>
@@ -5187,13 +5181,13 @@
         <v>2014</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E197" t="s">
         <v>204</v>
       </c>
       <c r="F197" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="96">
@@ -5204,13 +5198,13 @@
         <v>2014</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E198" t="s">
         <v>204</v>
       </c>
       <c r="F198" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="199" spans="1:6" ht="80">
@@ -5221,13 +5215,13 @@
         <v>2014</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E199" t="s">
         <v>204</v>
       </c>
       <c r="F199" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="200" spans="1:6" ht="64">
@@ -5238,7 +5232,7 @@
         <v>2014</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E200" t="s">
         <v>204</v>
@@ -5255,13 +5249,13 @@
         <v>2014</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E201" t="s">
         <v>204</v>
       </c>
       <c r="F201" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="202" spans="1:6" ht="80">
@@ -5272,7 +5266,7 @@
         <v>2015</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E202" t="s">
         <v>204</v>
@@ -5289,7 +5283,7 @@
         <v>2015</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E203" t="s">
         <v>203</v>
@@ -5306,13 +5300,13 @@
         <v>2015</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E204" t="s">
         <v>204</v>
       </c>
       <c r="F204" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="205" spans="1:6" ht="80">
@@ -5323,13 +5317,13 @@
         <v>2015</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E205" t="s">
         <v>204</v>
       </c>
       <c r="F205" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="206" spans="1:6" ht="64">
@@ -5340,7 +5334,7 @@
         <v>2015</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E206" t="s">
         <v>203</v>
@@ -5348,36 +5342,36 @@
     </row>
     <row r="207" spans="1:6" ht="80">
       <c r="A207" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B207">
         <v>2015</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E207" t="s">
         <v>227</v>
       </c>
       <c r="F207" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="208" spans="1:6" ht="48">
       <c r="A208" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B208">
         <v>2016</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E208" t="s">
         <v>227</v>
       </c>
       <c r="F208" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="209" spans="1:6" ht="96">
@@ -5388,13 +5382,13 @@
         <v>2015</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E209" t="s">
         <v>203</v>
       </c>
       <c r="F209" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="210" spans="1:6" ht="96">
@@ -5405,13 +5399,13 @@
         <v>2015</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E210" t="s">
         <v>204</v>
       </c>
       <c r="F210" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>